<commit_message>
errors estimations added + redistribution
</commit_message>
<xml_diff>
--- a/input/calorimetry/test_3.xlsx
+++ b/input/calorimetry/test_3.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KEVreplica\input\calorimetry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10896626-7FB3-4986-99E5-20A16344E3DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,8 @@
     <sheet name="targets" sheetId="6" r:id="rId6"/>
     <sheet name="enthalpies" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -120,11 +120,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,16 +436,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -473,7 +473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -487,7 +487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -501,7 +501,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -521,36 +521,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5.35</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7.34</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7.44</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9.4700000000000006</v>
       </c>
@@ -561,19 +561,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -584,7 +584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -598,7 +598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1.9109999999999999E-2</v>
       </c>
@@ -613,7 +613,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1.9650000000000001E-2</v>
       </c>
@@ -628,7 +628,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1.9109999999999999E-2</v>
       </c>
@@ -643,7 +643,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1.9650000000000001E-2</v>
       </c>
@@ -658,7 +658,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1.9109999999999999E-2</v>
       </c>
@@ -673,7 +673,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1.9650000000000001E-2</v>
       </c>
@@ -688,7 +688,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1.9109999999999999E-2</v>
       </c>
@@ -703,7 +703,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1.9650000000000001E-2</v>
       </c>
@@ -718,7 +718,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2.568E-3</v>
       </c>
@@ -733,7 +733,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3.4949999999999998E-3</v>
       </c>
@@ -748,7 +748,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2.568E-3</v>
       </c>
@@ -763,7 +763,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>3.4919999999999999E-3</v>
       </c>
@@ -777,7 +777,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2.568E-3</v>
       </c>
@@ -791,7 +791,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3.4940000000000001E-3</v>
       </c>
@@ -805,7 +805,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2.568E-3</v>
       </c>
@@ -819,7 +819,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>3.4949999999999998E-3</v>
       </c>
@@ -839,16 +839,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -859,16 +859,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -897,7 +897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -926,7 +926,7 @@
         <v>-9.8544999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -984,7 +984,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1019,16 +1019,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1039,16 +1039,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>-5.18</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>

</xml_diff>